<commit_message>
refactor ColorTransactions.xaml, CreateTransactionsData.xaml, 1c scripts locations, MatchSecondTransaction.xaml, FillResult.xaml issues
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>Data\Temp\Шаблон.xlsx</t>
+  </si>
+  <si>
+    <t>ResultsInputPath</t>
+  </si>
+  <si>
+    <t>Data\Input\Шаблон.xlsx</t>
   </si>
 </sst>
 </file>
@@ -576,7 +582,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -696,7 +702,14 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>